<commit_message>
Změna z amplitudy na poměrný útlum
</commit_message>
<xml_diff>
--- a/Keras_Sequential_data.xlsx
+++ b/Keras_Sequential_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,16 @@
           <t>mse_loss</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 10</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 11</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -524,6 +534,8 @@
       <c r="J2" t="n">
         <v>0.005569309927523136</v>
       </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -564,6 +576,8 @@
       <c r="J3" t="n">
         <v>0.003146809758618474</v>
       </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -604,6 +618,8 @@
       <c r="J4" t="n">
         <v>0.005345708224922419</v>
       </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -612,16 +628,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[36, 64, 128, 512, 128, 64, 1]</t>
+          <t>[128, 128, 1]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['relu', 'relu', 'relu', 'relu', 'relu', 'relu', 'linear']</t>
+          <t>['relu', 'relu', 'linear']</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -630,20 +646,22 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="G5" t="n">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="H5" t="n">
-        <v>2.642996215820312</v>
+        <v>0.3605457623799642</v>
       </c>
       <c r="I5" t="n">
-        <v>145.3647918701172</v>
+        <v>5.408186435699463</v>
       </c>
       <c r="J5" t="n">
-        <v>0.003096349770203233</v>
-      </c>
+        <v>11.92198085784912</v>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -652,16 +670,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>[36, 64, 128, 512, 128, 64, 1]</t>
+          <t>[128, 128, 1]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>['selu', 'selu', 'selu', 'selu', 'selu', 'selu', 'linear']</t>
+          <t>['relu', 'relu', 'linear']</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -670,20 +688,22 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="G6" t="n">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="H6" t="n">
-        <v>2.733361344127094</v>
+        <v>0.391872331693575</v>
       </c>
       <c r="I6" t="n">
-        <v>371.7371428012848</v>
+        <v>60.34833908081055</v>
       </c>
       <c r="J6" t="n">
-        <v>0.01195973809808493</v>
-      </c>
+        <v>4.974963188171387</v>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -692,16 +712,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>[36, 64, 128, 512, 128, 64, 1]</t>
+          <t>[128, 128, 1]</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>['selu', 'selu', 'selu', 'selu', 'selu', 'selu', 'linear']</t>
+          <t>['relu', 'relu', 'linear']</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -710,20 +730,22 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="G7" t="n">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="H7" t="n">
-        <v>3.117714087168376</v>
+        <v>0.4601679030497363</v>
       </c>
       <c r="I7" t="n">
-        <v>18.70628452301025</v>
+        <v>72.24636077880859</v>
       </c>
       <c r="J7" t="n">
-        <v>0.01014582253992558</v>
-      </c>
+        <v>2.854086399078369</v>
+      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -736,12 +758,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[512, 512, 1]</t>
+          <t>[128, 128, 1]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>['selu', 'selu', 'linear']</t>
+          <t>['relu', 'relu', 'linear']</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -750,20 +772,22 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>200</v>
+        <v>132</v>
       </c>
       <c r="G8" t="n">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="H8" t="n">
-        <v>5.221585512161255</v>
+        <v>0.3442076715556058</v>
       </c>
       <c r="I8" t="n">
-        <v>1044.317102432251</v>
+        <v>45.43541264533997</v>
       </c>
       <c r="J8" t="n">
-        <v>0.003163158660754561</v>
-      </c>
+        <v>0.3319054841995239</v>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -776,12 +800,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[512, 512, 1]</t>
+          <t>[128, 128, 1]</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>['selu', 'selu', 'linear']</t>
+          <t>['relu', 'relu', 'linear']</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -790,20 +814,22 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="G9" t="n">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="H9" t="n">
-        <v>3.375575995445252</v>
+        <v>0.9589118817273308</v>
       </c>
       <c r="I9" t="n">
-        <v>337.5575995445251</v>
+        <v>81.50750994682312</v>
       </c>
       <c r="J9" t="n">
-        <v>0.003904947778210044</v>
-      </c>
+        <v>0.004373230971395969</v>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -816,12 +842,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[512, 512, 1]</t>
+          <t>[128, 128, 1]</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>['selu', 'selu', 'linear']</t>
+          <t>['relu', 'relu', 'linear']</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -830,20 +856,22 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>200</v>
+        <v>69</v>
       </c>
       <c r="G10" t="n">
         <v>10000</v>
       </c>
       <c r="H10" t="n">
-        <v>0.516076431274414</v>
+        <v>0.7403726232224617</v>
       </c>
       <c r="I10" t="n">
-        <v>103.2152862548828</v>
+        <v>51.08571100234985</v>
       </c>
       <c r="J10" t="n">
-        <v>0.001804083818569779</v>
-      </c>
+        <v>35.91139602661133</v>
+      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -852,16 +880,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>[512, 512, 512, 512, 512, 1]</t>
+          <t>[128, 128, 1]</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>['selu', 'selu', 'selu', 'selu', 'selu', 'linear']</t>
+          <t>['relu', 'relu', 'linear']</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -870,20 +898,22 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="G11" t="n">
         <v>10000</v>
       </c>
       <c r="H11" t="n">
-        <v>0.8400297641754151</v>
+        <v>0.4907066553411349</v>
       </c>
       <c r="I11" t="n">
-        <v>84.0029764175415</v>
+        <v>34.84017252922058</v>
       </c>
       <c r="J11" t="n">
-        <v>0.0208949726074934</v>
-      </c>
+        <v>0.2965547144412994</v>
+      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -892,16 +922,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>[512, 512, 512, 512, 1]</t>
+          <t>[128, 128, 1]</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>['selu', 'selu', 'selu', 'selu', 'linear']</t>
+          <t>['relu', 'relu', 'linear']</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -910,19 +940,25 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>100</v>
+        <v>145</v>
       </c>
       <c r="G12" t="n">
         <v>10000</v>
       </c>
       <c r="H12" t="n">
-        <v>0.759941713809967</v>
+        <v>0.4851904753980966</v>
       </c>
       <c r="I12" t="n">
-        <v>75.9941713809967</v>
+        <v>70.352618932724</v>
       </c>
       <c r="J12" t="n">
-        <v>0.00497632659971714</v>
+        <v>1.613486165297218e-05</v>
+      </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>pozn F0 = 1N</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -932,16 +968,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>[512, 512, 512, 1]</t>
+          <t>[36, 64, 128, 512, 128, 64, 1]</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>['selu', 'selu', 'selu', 'linear']</t>
+          <t>['relu', 'relu', 'relu', 'relu', 'relu', 'relu', 'linear']</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -950,20 +986,22 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="G13" t="n">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="H13" t="n">
-        <v>0.6055253720283509</v>
+        <v>2.642996215820312</v>
       </c>
       <c r="I13" t="n">
-        <v>60.55253720283508</v>
+        <v>145.3647918701172</v>
       </c>
       <c r="J13" t="n">
-        <v>0.002790062455460429</v>
-      </c>
+        <v>0.003096349770203233</v>
+      </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -972,16 +1010,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>[64, 64, 1]</t>
+          <t>[36, 64, 128, 512, 128, 64, 1]</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>['selu', 'selu', 'linear']</t>
+          <t>['selu', 'selu', 'selu', 'selu', 'selu', 'selu', 'linear']</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -990,20 +1028,22 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="G14" t="n">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="H14" t="n">
-        <v>0.4843237280845642</v>
+        <v>2.733361344127094</v>
       </c>
       <c r="I14" t="n">
-        <v>48.43237280845642</v>
+        <v>371.7371428012848</v>
       </c>
       <c r="J14" t="n">
-        <v>0.004352561663836241</v>
-      </c>
+        <v>0.01195973809808493</v>
+      </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1012,16 +1052,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>[128, 128, 1]</t>
+          <t>[36, 64, 128, 512, 128, 64, 1]</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>['selu', 'selu', 'linear']</t>
+          <t>['selu', 'selu', 'selu', 'selu', 'selu', 'selu', 'linear']</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1030,20 +1070,22 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="G15" t="n">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="H15" t="n">
-        <v>0.4962827444076538</v>
+        <v>3.117714087168376</v>
       </c>
       <c r="I15" t="n">
-        <v>49.62827444076538</v>
+        <v>18.70628452301025</v>
       </c>
       <c r="J15" t="n">
-        <v>0.00113097857683897</v>
-      </c>
+        <v>0.01014582253992558</v>
+      </c>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1056,7 +1098,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>[256, 256, 1]</t>
+          <t>[512, 512, 1]</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1070,20 +1112,22 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G16" t="n">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="H16" t="n">
-        <v>0.537766580581665</v>
+        <v>5.221585512161255</v>
       </c>
       <c r="I16" t="n">
-        <v>53.7766580581665</v>
+        <v>1044.317102432251</v>
       </c>
       <c r="J16" t="n">
-        <v>0.003508876776322722</v>
-      </c>
+        <v>0.003163158660754561</v>
+      </c>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1113,17 +1157,19 @@
         <v>100</v>
       </c>
       <c r="G17" t="n">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="H17" t="n">
-        <v>0.7661984515190124</v>
+        <v>3.375575995445252</v>
       </c>
       <c r="I17" t="n">
-        <v>76.61984515190125</v>
+        <v>337.5575995445251</v>
       </c>
       <c r="J17" t="n">
-        <v>0.001072098850272596</v>
-      </c>
+        <v>0.003904947778210044</v>
+      </c>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1136,7 +1182,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>[1028, 1028, 1]</t>
+          <t>[512, 512, 1]</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1150,20 +1196,22 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G18" t="n">
         <v>10000</v>
       </c>
       <c r="H18" t="n">
-        <v>1.335580596923828</v>
+        <v>0.516076431274414</v>
       </c>
       <c r="I18" t="n">
-        <v>133.5580596923828</v>
+        <v>103.2152862548828</v>
       </c>
       <c r="J18" t="n">
-        <v>0.01241711713373661</v>
-      </c>
+        <v>0.001804083818569779</v>
+      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1172,16 +1220,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>[1028, 1028, 1]</t>
+          <t>[512, 512, 512, 512, 512, 1]</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>['relu', 'relu', 'linear']</t>
+          <t>['selu', 'selu', 'selu', 'selu', 'selu', 'linear']</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1196,14 +1244,16 @@
         <v>10000</v>
       </c>
       <c r="H19" t="n">
-        <v>1.270974922180176</v>
+        <v>0.8400297641754151</v>
       </c>
       <c r="I19" t="n">
-        <v>127.0974922180176</v>
+        <v>84.0029764175415</v>
       </c>
       <c r="J19" t="n">
-        <v>0.007752176374197006</v>
-      </c>
+        <v>0.0208949726074934</v>
+      </c>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1212,16 +1262,16 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>[64, 64, 1]</t>
+          <t>[512, 512, 512, 512, 1]</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>['relu', 'relu', 'linear']</t>
+          <t>['selu', 'selu', 'selu', 'selu', 'linear']</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1236,14 +1286,16 @@
         <v>10000</v>
       </c>
       <c r="H20" t="n">
-        <v>0.4836410164833069</v>
+        <v>0.759941713809967</v>
       </c>
       <c r="I20" t="n">
-        <v>48.36410164833069</v>
+        <v>75.9941713809967</v>
       </c>
       <c r="J20" t="n">
-        <v>0.001767968875356019</v>
-      </c>
+        <v>0.00497632659971714</v>
+      </c>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1252,16 +1304,16 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>[128, 128, 1]</t>
+          <t>[512, 512, 512, 1]</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>['relu', 'relu', 'linear']</t>
+          <t>['selu', 'selu', 'selu', 'linear']</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1276,14 +1328,16 @@
         <v>10000</v>
       </c>
       <c r="H21" t="n">
-        <v>0.481656379699707</v>
+        <v>0.6055253720283509</v>
       </c>
       <c r="I21" t="n">
-        <v>48.1656379699707</v>
+        <v>60.55253720283508</v>
       </c>
       <c r="J21" t="n">
-        <v>0.002778570400550961</v>
-      </c>
+        <v>0.002790062455460429</v>
+      </c>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1296,12 +1350,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>[512, 512, 1]</t>
+          <t>[64, 64, 1]</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>['relu', 'relu', 'linear']</t>
+          <t>['selu', 'selu', 'linear']</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1316,14 +1370,16 @@
         <v>10000</v>
       </c>
       <c r="H22" t="n">
-        <v>0.711573977470398</v>
+        <v>0.4843237280845642</v>
       </c>
       <c r="I22" t="n">
-        <v>71.15739774703979</v>
+        <v>48.43237280845642</v>
       </c>
       <c r="J22" t="n">
-        <v>0.02799069322645664</v>
-      </c>
+        <v>0.004352561663836241</v>
+      </c>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1336,12 +1392,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>[2056, 2056, 1]</t>
+          <t>[128, 128, 1]</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>['sigmoid', 'sigmoid', 'linear']</t>
+          <t>['selu', 'selu', 'linear']</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1356,14 +1412,16 @@
         <v>10000</v>
       </c>
       <c r="H23" t="n">
-        <v>2.341329197883606</v>
+        <v>0.4962827444076538</v>
       </c>
       <c r="I23" t="n">
-        <v>234.1329197883606</v>
+        <v>49.62827444076538</v>
       </c>
       <c r="J23" t="n">
-        <v>0.004292678087949753</v>
-      </c>
+        <v>0.00113097857683897</v>
+      </c>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1376,12 +1434,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>[1028, 1028, 1]</t>
+          <t>[256, 256, 1]</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>['sigmoid', 'sigmoid', 'linear']</t>
+          <t>['selu', 'selu', 'linear']</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1396,14 +1454,16 @@
         <v>10000</v>
       </c>
       <c r="H24" t="n">
-        <v>1.319502077102661</v>
+        <v>0.537766580581665</v>
       </c>
       <c r="I24" t="n">
-        <v>131.9502077102661</v>
+        <v>53.7766580581665</v>
       </c>
       <c r="J24" t="n">
-        <v>0.007079277653247118</v>
-      </c>
+        <v>0.003508876776322722</v>
+      </c>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1416,12 +1476,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>[64, 64, 1]</t>
+          <t>[512, 512, 1]</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>['sigmoid', 'sigmoid', 'linear']</t>
+          <t>['selu', 'selu', 'linear']</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1436,14 +1496,16 @@
         <v>10000</v>
       </c>
       <c r="H25" t="n">
-        <v>0.4893174386024475</v>
+        <v>0.7661984515190124</v>
       </c>
       <c r="I25" t="n">
-        <v>48.93174386024475</v>
+        <v>76.61984515190125</v>
       </c>
       <c r="J25" t="n">
-        <v>0.003201575949788094</v>
-      </c>
+        <v>0.001072098850272596</v>
+      </c>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1456,12 +1518,12 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>[128, 128, 1]</t>
+          <t>[1028, 1028, 1]</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>['sigmoid', 'sigmoid', 'linear']</t>
+          <t>['selu', 'selu', 'linear']</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1476,14 +1538,352 @@
         <v>10000</v>
       </c>
       <c r="H26" t="n">
+        <v>1.335580596923828</v>
+      </c>
+      <c r="I26" t="n">
+        <v>133.5580596923828</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.01241711713373661</v>
+      </c>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>StandardScaler</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>3</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>[1028, 1028, 1]</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>['relu', 'relu', 'linear']</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Adam</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>100</v>
+      </c>
+      <c r="G27" t="n">
+        <v>10000</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1.270974922180176</v>
+      </c>
+      <c r="I27" t="n">
+        <v>127.0974922180176</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.007752176374197006</v>
+      </c>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>StandardScaler</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>3</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>[64, 64, 1]</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>['relu', 'relu', 'linear']</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Adam</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>100</v>
+      </c>
+      <c r="G28" t="n">
+        <v>10000</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.4836410164833069</v>
+      </c>
+      <c r="I28" t="n">
+        <v>48.36410164833069</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.001767968875356019</v>
+      </c>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>StandardScaler</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>3</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>[128, 128, 1]</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>['relu', 'relu', 'linear']</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Adam</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>100</v>
+      </c>
+      <c r="G29" t="n">
+        <v>10000</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.481656379699707</v>
+      </c>
+      <c r="I29" t="n">
+        <v>48.1656379699707</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.002778570400550961</v>
+      </c>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>StandardScaler</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>3</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>[512, 512, 1]</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>['relu', 'relu', 'linear']</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Adam</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>100</v>
+      </c>
+      <c r="G30" t="n">
+        <v>10000</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.711573977470398</v>
+      </c>
+      <c r="I30" t="n">
+        <v>71.15739774703979</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.02799069322645664</v>
+      </c>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>StandardScaler</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>3</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>[2056, 2056, 1]</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>['sigmoid', 'sigmoid', 'linear']</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Adam</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>100</v>
+      </c>
+      <c r="G31" t="n">
+        <v>10000</v>
+      </c>
+      <c r="H31" t="n">
+        <v>2.341329197883606</v>
+      </c>
+      <c r="I31" t="n">
+        <v>234.1329197883606</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.004292678087949753</v>
+      </c>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>StandardScaler</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>3</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>[1028, 1028, 1]</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>['sigmoid', 'sigmoid', 'linear']</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Adam</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>100</v>
+      </c>
+      <c r="G32" t="n">
+        <v>10000</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1.319502077102661</v>
+      </c>
+      <c r="I32" t="n">
+        <v>131.9502077102661</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.007079277653247118</v>
+      </c>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>StandardScaler</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>3</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>[64, 64, 1]</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>['sigmoid', 'sigmoid', 'linear']</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Adam</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>100</v>
+      </c>
+      <c r="G33" t="n">
+        <v>10000</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.4893174386024475</v>
+      </c>
+      <c r="I33" t="n">
+        <v>48.93174386024475</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.003201575949788094</v>
+      </c>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>StandardScaler</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>3</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>[128, 128, 1]</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>['sigmoid', 'sigmoid', 'linear']</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Adam</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>100</v>
+      </c>
+      <c r="G34" t="n">
+        <v>10000</v>
+      </c>
+      <c r="H34" t="n">
         <v>0.4915751028060913</v>
       </c>
-      <c r="I26" t="n">
+      <c r="I34" t="n">
         <v>49.15751028060913</v>
       </c>
-      <c r="J26" t="n">
+      <c r="J34" t="n">
         <v>0.004622235428541899</v>
       </c>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>